<commit_message>
Minor changes for chart addition
</commit_message>
<xml_diff>
--- a/Test Case - 3/TC3_Results_C.xlsx
+++ b/Test Case - 3/TC3_Results_C.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -893,21 +893,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -953,7 +953,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -986,6 +986,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1001,6 +1011,86 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1290,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q109"/>
+  <dimension ref="A1:R109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O95" sqref="O95"/>
+      <selection activeCell="Q84" sqref="Q84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,81 +1391,83 @@
     <col min="8" max="8" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="4" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1421,11 +1513,11 @@
       <c r="O3">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1471,11 +1563,11 @@
       <c r="O4">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1521,11 +1613,11 @@
       <c r="O5">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1571,11 +1663,11 @@
       <c r="O6">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1621,11 +1713,11 @@
       <c r="O7">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1671,11 +1763,11 @@
       <c r="O8">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1721,11 +1813,11 @@
       <c r="O9">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1771,11 +1863,11 @@
       <c r="O10">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1821,11 +1913,11 @@
       <c r="O11">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1871,11 +1963,11 @@
       <c r="O12">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1921,11 +2013,11 @@
       <c r="O13">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1971,11 +2063,11 @@
       <c r="O14">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2021,11 +2113,11 @@
       <c r="O15">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2071,11 +2163,11 @@
       <c r="O16">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2121,11 +2213,11 @@
       <c r="O17">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2171,11 +2263,11 @@
       <c r="O18">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2221,11 +2313,11 @@
       <c r="O19">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2271,11 +2363,11 @@
       <c r="O20">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2321,11 +2413,11 @@
       <c r="O21">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2371,11 +2463,11 @@
       <c r="O22">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2421,11 +2513,11 @@
       <c r="O23">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2462,11 +2554,11 @@
       <c r="L24" t="b">
         <v>0</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2512,11 +2604,11 @@
       <c r="O25">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2562,11 +2654,11 @@
       <c r="O26">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2612,11 +2704,11 @@
       <c r="O27">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2662,11 +2754,11 @@
       <c r="O28">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2712,11 +2804,11 @@
       <c r="O29">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2762,11 +2854,11 @@
       <c r="O30">
         <v>30.152000000000001</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2812,11 +2904,11 @@
       <c r="O31">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2862,11 +2954,11 @@
       <c r="O32">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2912,11 +3004,11 @@
       <c r="O33">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="R33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2962,15 +3054,18 @@
       <c r="O34">
         <v>35.152000000000001</v>
       </c>
-      <c r="P34" s="7">
+      <c r="P34" s="4">
         <f>0.9*((O34-D34)^0.51)*((SQRT((M34-B34)^2+(N34-C34)^2)^(-0.35)))</f>
         <v>1.486934389517961</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="Q34" t="b">
+        <v>1</v>
+      </c>
+      <c r="R34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3007,11 +3102,11 @@
       <c r="L35" t="b">
         <v>0</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="R35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3057,11 +3152,11 @@
       <c r="O36">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="R36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3107,11 +3202,11 @@
       <c r="O37">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="R37" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3157,11 +3252,11 @@
       <c r="O38">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3207,11 +3302,11 @@
       <c r="O39">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="R39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3257,11 +3352,11 @@
       <c r="O40">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="R40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3307,11 +3402,11 @@
       <c r="O41">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="R41" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3357,11 +3452,11 @@
       <c r="O42">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="R42" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3407,15 +3502,18 @@
       <c r="O43">
         <v>35.152000000000001</v>
       </c>
-      <c r="P43" s="7">
+      <c r="P43" s="4">
         <f>0.9*((O43-D43)^0.51)*((SQRT((M43-B43)^2+(N43-C43)^2)^(-0.35)))</f>
         <v>1.1644085258098895</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="Q43" t="b">
+        <v>1</v>
+      </c>
+      <c r="R43" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3461,15 +3559,18 @@
       <c r="O44">
         <v>35.152000000000001</v>
       </c>
-      <c r="P44" s="7">
+      <c r="P44" s="4">
         <f>0.9*((O44-D44)^0.51)*((SQRT((M44-B44)^2+(N44-C44)^2)^(-0.35)))</f>
         <v>1.4896628100405325</v>
       </c>
-      <c r="Q44" t="s">
+      <c r="Q44" t="b">
+        <v>1</v>
+      </c>
+      <c r="R44" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3515,11 +3616,11 @@
       <c r="O45">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q45" t="s">
+      <c r="R45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3565,11 +3666,11 @@
       <c r="O46">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q46" t="s">
+      <c r="R46" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3615,11 +3716,11 @@
       <c r="O47">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="R47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3665,11 +3766,11 @@
       <c r="O48">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q48" t="s">
+      <c r="R48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3715,11 +3816,11 @@
       <c r="O49">
         <v>35.152000000000001</v>
       </c>
-      <c r="Q49" t="s">
+      <c r="R49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3765,11 +3866,11 @@
       <c r="O50">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="R50" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3815,11 +3916,11 @@
       <c r="O51">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q51" t="s">
+      <c r="R51" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3865,11 +3966,11 @@
       <c r="O52">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q52" t="s">
+      <c r="R52" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3915,11 +4016,11 @@
       <c r="O53">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q53" t="s">
+      <c r="R53" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3965,11 +4066,11 @@
       <c r="O54">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q54" t="s">
+      <c r="R54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4015,11 +4116,11 @@
       <c r="O55">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q55" t="s">
+      <c r="R55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4065,11 +4166,11 @@
       <c r="O56">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q56" t="s">
+      <c r="R56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4115,11 +4216,11 @@
       <c r="O57">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q57" t="s">
+      <c r="R57" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4165,11 +4266,11 @@
       <c r="O58">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q58" t="s">
+      <c r="R58" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4215,11 +4316,11 @@
       <c r="O59">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q59" t="s">
+      <c r="R59" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4265,11 +4366,11 @@
       <c r="O60">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q60" t="s">
+      <c r="R60" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4315,11 +4416,11 @@
       <c r="O61">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q61" t="s">
+      <c r="R61" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4365,11 +4466,11 @@
       <c r="O62">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q62" t="s">
+      <c r="R62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4415,11 +4516,11 @@
       <c r="O63">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q63" t="s">
+      <c r="R63" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4465,11 +4566,11 @@
       <c r="O64">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q64" t="s">
+      <c r="R64" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4515,11 +4616,11 @@
       <c r="O65">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q65" t="s">
+      <c r="R65" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4565,11 +4666,11 @@
       <c r="O66">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q66" t="s">
+      <c r="R66" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4615,11 +4716,11 @@
       <c r="O67">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q67" t="s">
+      <c r="R67" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4665,11 +4766,11 @@
       <c r="O68">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q68" t="s">
+      <c r="R68" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4715,11 +4816,11 @@
       <c r="O69">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q69" t="s">
+      <c r="R69" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4765,11 +4866,11 @@
       <c r="O70">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q70" t="s">
+      <c r="R70" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4815,11 +4916,11 @@
       <c r="O71">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q71" t="s">
+      <c r="R71" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4865,11 +4966,11 @@
       <c r="O72">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q72" t="s">
+      <c r="R72" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4915,11 +5016,11 @@
       <c r="O73">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q73" t="s">
+      <c r="R73" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4965,11 +5066,11 @@
       <c r="O74">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q74" t="s">
+      <c r="R74" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5015,11 +5116,11 @@
       <c r="O75">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q75" t="s">
+      <c r="R75" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5065,11 +5166,11 @@
       <c r="O76">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q76" t="s">
+      <c r="R76" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5115,11 +5216,11 @@
       <c r="O77">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q77" t="s">
+      <c r="R77" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5165,11 +5266,11 @@
       <c r="O78">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q78" t="s">
+      <c r="R78" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5215,11 +5316,11 @@
       <c r="O79">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q79" t="s">
+      <c r="R79" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5265,11 +5366,11 @@
       <c r="O80">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q80" t="s">
+      <c r="R80" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5315,11 +5416,11 @@
       <c r="O81">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q81" t="s">
+      <c r="R81" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5365,11 +5466,11 @@
       <c r="O82">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q82" t="s">
+      <c r="R82" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5415,11 +5516,11 @@
       <c r="O83">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q83" t="s">
+      <c r="R83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5465,15 +5566,18 @@
       <c r="O84">
         <v>37.652000000000001</v>
       </c>
-      <c r="P84" s="7">
+      <c r="P84" s="4">
         <f>0.9*((O84-D84)^0.51)*((SQRT((M84-B84)^2+(N84-C84)^2)^(-0.35)))</f>
         <v>0.93101418279599779</v>
       </c>
-      <c r="Q84" t="s">
+      <c r="Q84" t="b">
+        <v>1</v>
+      </c>
+      <c r="R84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5519,11 +5623,11 @@
       <c r="O85">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q85" t="s">
+      <c r="R85" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5569,11 +5673,11 @@
       <c r="O86">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q86" t="s">
+      <c r="R86" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5619,11 +5723,11 @@
       <c r="O87">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q87" t="s">
+      <c r="R87" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5669,11 +5773,11 @@
       <c r="O88">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q88" t="s">
+      <c r="R88" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5719,11 +5823,11 @@
       <c r="O89">
         <v>37.652000000000001</v>
       </c>
-      <c r="Q89" t="s">
+      <c r="R89" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5760,11 +5864,11 @@
       <c r="L90" t="b">
         <v>1</v>
       </c>
-      <c r="Q90" t="s">
+      <c r="R90" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5801,11 +5905,11 @@
       <c r="L91" t="b">
         <v>1</v>
       </c>
-      <c r="Q91" t="s">
+      <c r="R91" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5842,11 +5946,11 @@
       <c r="L92" t="b">
         <v>1</v>
       </c>
-      <c r="Q92" t="s">
+      <c r="R92" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5880,11 +5984,11 @@
       <c r="L93" t="b">
         <v>1</v>
       </c>
-      <c r="Q93" t="s">
+      <c r="R93" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5918,11 +6022,11 @@
       <c r="L94" t="b">
         <v>1</v>
       </c>
-      <c r="Q94" t="s">
+      <c r="R94" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5956,11 +6060,11 @@
       <c r="L95" t="b">
         <v>1</v>
       </c>
-      <c r="Q95" t="s">
+      <c r="R95" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5994,11 +6098,11 @@
       <c r="L96" t="b">
         <v>1</v>
       </c>
-      <c r="Q96" t="s">
+      <c r="R96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6032,11 +6136,11 @@
       <c r="L97" t="b">
         <v>1</v>
       </c>
-      <c r="Q97" t="s">
+      <c r="R97" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6070,11 +6174,11 @@
       <c r="L98" t="b">
         <v>1</v>
       </c>
-      <c r="Q98" t="s">
+      <c r="R98" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6108,11 +6212,11 @@
       <c r="L99" t="b">
         <v>0</v>
       </c>
-      <c r="Q99" t="s">
+      <c r="R99" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6146,11 +6250,11 @@
       <c r="L100" t="b">
         <v>1</v>
       </c>
-      <c r="Q100" t="s">
+      <c r="R100" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6184,11 +6288,11 @@
       <c r="L101" t="b">
         <v>1</v>
       </c>
-      <c r="Q101" t="s">
+      <c r="R101" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6222,11 +6326,11 @@
       <c r="L102" t="b">
         <v>1</v>
       </c>
-      <c r="Q102" t="s">
+      <c r="R102" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -6260,11 +6364,11 @@
       <c r="L103" t="b">
         <v>1</v>
       </c>
-      <c r="Q103" t="s">
+      <c r="R103" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6298,11 +6402,11 @@
       <c r="L104" t="b">
         <v>1</v>
       </c>
-      <c r="Q104" t="s">
+      <c r="R104" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -6336,11 +6440,11 @@
       <c r="L105" t="b">
         <v>1</v>
       </c>
-      <c r="Q105" t="s">
+      <c r="R105" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -6374,11 +6478,11 @@
       <c r="L106" t="b">
         <v>1</v>
       </c>
-      <c r="Q106" t="s">
+      <c r="R106" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -6412,11 +6516,11 @@
       <c r="L107" t="b">
         <v>1</v>
       </c>
-      <c r="Q107" t="s">
+      <c r="R107" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -6450,11 +6554,11 @@
       <c r="L108" t="b">
         <v>1</v>
       </c>
-      <c r="Q108" t="s">
+      <c r="R108" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -6488,12 +6592,16 @@
       <c r="L109" t="b">
         <v>1</v>
       </c>
-      <c r="Q109" t="s">
+      <c r="R109" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="I1:I2"/>
@@ -6501,12 +6609,52 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L109">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q34">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q43">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q44">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q84">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>

</xml_diff>